<commit_message>
Registration, Login and Authentication implemented
</commit_message>
<xml_diff>
--- a/Documents/Design/WebAPI_Routes.xlsx
+++ b/Documents/Design/WebAPI_Routes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -76,6 +76,83 @@
   <si>
     <t>{
 authToken: &lt;string&gt;
+}
+or 
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>Auth-token required ?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no, generates and returns it if credentials were correct</t>
+  </si>
+  <si>
+    <t>{
+}</t>
+  </si>
+  <si>
+    <t>OK 200
+or
+errorCode</t>
+  </si>
+  <si>
+    <t>ResponseHeader</t>
+  </si>
+  <si>
+    <t>none
+or
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>Created 201
+or
+errorCode</t>
+  </si>
+  <si>
+    <t>{
+username: &lt;string&gt;,
+password: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>yes, invalidates the given auth token if correct</t>
+  </si>
+  <si>
+    <t>{
+value=&lt;number&gt;
+}</t>
+  </si>
+  <si>
+    <t>/highscore/{userId}/level/{levelIndex}</t>
+  </si>
+  <si>
+    <t>{
+'&lt;number (index)&gt;' : &lt;number&gt; (highscore)
+}
+or
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>{
+user:{
+id: &lt;number&gt;,
+username: &lt;string&gt;,
+}
 }
 or 
 {
@@ -134,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -142,6 +219,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,21 +543,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,13 +570,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -498,10 +592,20 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -511,12 +615,20 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
       <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -526,10 +638,18 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="2"/>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -537,12 +657,20 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="2"/>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -550,10 +678,39 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished Serverside of WebAPI. Clientside Login and Logout done.
</commit_message>
<xml_diff>
--- a/Documents/Design/WebAPI_Routes.xlsx
+++ b/Documents/Design/WebAPI_Routes.xlsx
@@ -96,10 +96,6 @@
     <t>no, generates and returns it if credentials were correct</t>
   </si>
   <si>
-    <t>{
-}</t>
-  </si>
-  <si>
     <t>OK 200
 or
 errorCode</t>
@@ -136,16 +132,6 @@
   </si>
   <si>
     <t>/highscore/{userId}/level/{levelIndex}</t>
-  </si>
-  <si>
-    <t>{
-'&lt;number (index)&gt;' : &lt;number&gt; (highscore)
-}
-or
-{
-errorCode: &lt;number&gt;,
-errorMessage: &lt;string&gt;
-}</t>
   </si>
   <si>
     <t>{
@@ -158,6 +144,21 @@
 {
 errorCode: &lt;number&gt;,
 errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>{
+'&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
+}
+or
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
+    <t>{
+'&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
 }</t>
   </si>
 </sst>
@@ -545,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -596,13 +597,13 @@
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -619,10 +620,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>16</v>
@@ -639,14 +640,14 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -657,17 +658,17 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -678,20 +679,20 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -706,7 +707,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Fixed errors in web api and added the option to read rankings for a specific level from the database
</commit_message>
<xml_diff>
--- a/Documents/Design/WebAPI_Routes.xlsx
+++ b/Documents/Design/WebAPI_Routes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,31 @@
     <t>{
 '&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
 }</t>
+  </si>
+  <si>
+    <t>OK 200,
+or
+errorCode</t>
+  </si>
+  <si>
+    <t>OK 200 (No error, but old value was higher),
+CREATED 201 (New highscore stored)
+or
+errorCode</t>
+  </si>
+  <si>
+    <t>GetRanking</t>
+  </si>
+  <si>
+    <t>{
+&lt;number (index)&gt; : {
+username: &lt;string&gt;,
+value: &lt;number&gt;
+}
+}</t>
+  </si>
+  <si>
+    <t>/ranking/{levelIndex}[?limit={maxNumberOfResults}]</t>
   </si>
 </sst>
 </file>
@@ -212,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -229,6 +254,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,16 +572,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" style="6" customWidth="1"/>
@@ -671,7 +699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -688,7 +716,7 @@
         <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -711,6 +739,26 @@
       </c>
       <c r="G7" s="3" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional design content
</commit_message>
<xml_diff>
--- a/Documents/Design/WebAPI_Routes.xlsx
+++ b/Documents/Design/WebAPI_Routes.xlsx
@@ -74,16 +74,6 @@
     <t>/highscore/{userId}</t>
   </si>
   <si>
-    <t>{
-authToken: &lt;string&gt;
-}
-or 
-{
-errorCode: &lt;number&gt;,
-errorMessage: &lt;string&gt;
-}</t>
-  </si>
-  <si>
     <t>Auth-token required ?</t>
   </si>
   <si>
@@ -96,25 +86,7 @@
     <t>no, generates and returns it if credentials were correct</t>
   </si>
   <si>
-    <t>OK 200
-or
-errorCode</t>
-  </si>
-  <si>
     <t>ResponseHeader</t>
-  </si>
-  <si>
-    <t>none
-or
-{
-errorCode: &lt;number&gt;,
-errorMessage: &lt;string&gt;
-}</t>
-  </si>
-  <si>
-    <t>Created 201
-or
-errorCode</t>
   </si>
   <si>
     <t>{
@@ -132,6 +104,41 @@
   </si>
   <si>
     <t>/highscore/{userId}/level/{levelIndex}</t>
+  </si>
+  <si>
+    <t>{
+'&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
+}</t>
+  </si>
+  <si>
+    <t>GetRanking</t>
+  </si>
+  <si>
+    <t>{
+&lt;number (index)&gt; : {
+username: &lt;string&gt;,
+value: &lt;number&gt;
+}
+}</t>
+  </si>
+  <si>
+    <t>/ranking/{levelIndex}[?limit={maxNumberOfResults}]</t>
+  </si>
+  <si>
+    <t>OK 200 (No error, but old value was higher),
+CREATED 201 (New highscore stored)
+-OR-
+errorCode</t>
+  </si>
+  <si>
+    <t>OK 200
+-OR-
+errorCode</t>
+  </si>
+  <si>
+    <t>Created 201
+-OR-
+errorCode</t>
   </si>
   <si>
     <t>{
@@ -140,7 +147,7 @@
 username: &lt;string&gt;,
 }
 }
-or 
+-OR-
 {
 errorCode: &lt;number&gt;,
 errorMessage: &lt;string&gt;
@@ -148,43 +155,36 @@
   </si>
   <si>
     <t>{
-'&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
+authToken: &lt;string&gt;
 }
-or
+-OR-
 {
 errorCode: &lt;number&gt;,
 errorMessage: &lt;string&gt;
 }</t>
   </si>
   <si>
+    <t>none
+-OR-
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
+}</t>
+  </si>
+  <si>
     <t>{
 '&lt;number (levelIndex)&gt;' : &lt;number&gt; (highscore)
+}
+-OR-
+{
+errorCode: &lt;number&gt;,
+errorMessage: &lt;string&gt;
 }</t>
   </si>
   <si>
     <t>OK 200,
-or
+-OR-
 errorCode</t>
-  </si>
-  <si>
-    <t>OK 200 (No error, but old value was higher),
-CREATED 201 (New highscore stored)
-or
-errorCode</t>
-  </si>
-  <si>
-    <t>GetRanking</t>
-  </si>
-  <si>
-    <t>{
-&lt;number (index)&gt; : {
-username: &lt;string&gt;,
-value: &lt;number&gt;
-}
-}</t>
-  </si>
-  <si>
-    <t>/ranking/{levelIndex}[?limit={maxNumberOfResults}]</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,19 +599,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -622,19 +622,19 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -645,19 +645,19 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -668,14 +668,14 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -686,20 +686,20 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -707,20 +707,20 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -731,34 +731,34 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="G8" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional appendices to Assessment_01 document
</commit_message>
<xml_diff>
--- a/Documents/Design/WebAPI_Routes.xlsx
+++ b/Documents/Design/WebAPI_Routes.xlsx
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>